<commit_message>
Added some notes in the excel
</commit_message>
<xml_diff>
--- a/Design-part/UX diagram part A1 HYP design in the small and abstract pages.xlsx
+++ b/Design-part/UX diagram part A1 HYP design in the small and abstract pages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/040c5279d0540352/Documenti/Hypermedia Applications/Final Project/Design-part/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carloambrogi/Desktop/Hypermedia-Project/Design-part/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{F4E6931B-AF2C-1C48-A006-7C14552431DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29C31201-7A77-4698-98BC-4347DBF9C927}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA747284-1ED0-1345-8856-C614941FF4DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{CF35C348-60D3-C34C-B3F9-EC827BB88FFA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{CF35C348-60D3-C34C-B3F9-EC827BB88FFA}"/>
   </bookViews>
   <sheets>
     <sheet name="Content tables" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="86">
   <si>
     <t>Topic: "Town"</t>
   </si>
@@ -282,6 +282,18 @@
   </si>
   <si>
     <t>idem come sopra</t>
+  </si>
+  <si>
+    <t>Colonna1</t>
+  </si>
+  <si>
+    <t>sceglere come rappresentarlo</t>
+  </si>
+  <si>
+    <t>Title: Service type name</t>
+  </si>
+  <si>
+    <t>questo sarà la prewiew per il group link</t>
   </si>
 </sst>
 </file>
@@ -327,7 +339,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -384,11 +396,12 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{6DDB3FB5-D071-4A32-885B-8B86FDD5FAC8}" name="Table15" displayName="Table15" ref="A16:B27" totalsRowShown="0">
-  <autoFilter ref="A16:B27" xr:uid="{6DDB3FB5-D071-4A32-885B-8B86FDD5FAC8}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{6DDB3FB5-D071-4A32-885B-8B86FDD5FAC8}" name="Table15" displayName="Table15" ref="A16:C27" totalsRowShown="0">
+  <autoFilter ref="A16:C27" xr:uid="{6DDB3FB5-D071-4A32-885B-8B86FDD5FAC8}"/>
+  <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{CF67C389-C2D4-43D6-94BF-7AF9744F66FC}" name="Page for kind of topic: &quot;Events&quot;"/>
     <tableColumn id="2" xr3:uid="{8DE05ECF-AB8D-417E-BC77-E1ABEBC32636}" name="Column1"/>
+    <tableColumn id="3" xr3:uid="{54EFB7B2-58F8-CB45-982E-CEFA45CD2EFE}" name="Column2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -527,10 +540,11 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A66A5AF2-B58F-4EFE-BBF0-A9C7E6F124D6}" name="Table7" displayName="Table7" ref="A27:A29" totalsRowShown="0">
-  <autoFilter ref="A27:A29" xr:uid="{A66A5AF2-B58F-4EFE-BBF0-A9C7E6F124D6}"/>
-  <tableColumns count="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A66A5AF2-B58F-4EFE-BBF0-A9C7E6F124D6}" name="Table7" displayName="Table7" ref="A27:B29" totalsRowShown="0">
+  <autoFilter ref="A27:B29" xr:uid="{A66A5AF2-B58F-4EFE-BBF0-A9C7E6F124D6}"/>
+  <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{D162CF21-5F29-4B11-9384-455A4BE78ACA}" name="Kind of topic &quot;Services type&quot;"/>
+    <tableColumn id="2" xr3:uid="{C5742220-14CA-574E-A206-CAE6B6D2F1A6}" name="Colonna1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -577,7 +591,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -873,228 +887,234 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7009AE2-141B-8F43-BF6B-7E6ECFF7233C}">
-  <dimension ref="A1:A53"/>
+  <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="171" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="74.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>36</v>
       </c>
@@ -1121,17 +1141,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F52FC61-8669-774A-ACF5-BEF7FABCEB04}">
   <dimension ref="A1:C125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E119" sqref="E119"/>
+    <sheetView zoomScale="125" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="65.1640625" customWidth="1"/>
     <col min="2" max="2" width="62.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -1139,7 +1159,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -1147,27 +1167,27 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -1175,27 +1195,27 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1203,25 +1223,28 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>50</v>
       </c>
       <c r="B16" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -1229,22 +1252,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -1252,27 +1275,27 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>49</v>
       </c>
@@ -1280,15 +1303,18 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>52</v>
       </c>
       <c r="B27" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -1296,7 +1322,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -1304,22 +1330,22 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -1327,27 +1353,27 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>49</v>
       </c>
@@ -1355,7 +1381,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -1363,12 +1389,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>57</v>
       </c>
@@ -1376,7 +1402,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>38</v>
       </c>
@@ -1384,27 +1410,27 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>40</v>
       </c>
@@ -1412,27 +1438,27 @@
         <v>41</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>49</v>
       </c>
@@ -1440,7 +1466,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>52</v>
       </c>
@@ -1448,7 +1474,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>59</v>
       </c>
@@ -1459,20 +1485,20 @@
         <v>78</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>38</v>
       </c>
       <c r="B58" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>40</v>
       </c>
@@ -1480,22 +1506,22 @@
         <v>41</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
         <v>75</v>
       </c>
@@ -1503,7 +1529,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>49</v>
       </c>
@@ -1514,7 +1540,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>60</v>
       </c>
@@ -1522,7 +1548,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>38</v>
       </c>
@@ -1530,12 +1556,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>40</v>
       </c>
@@ -1543,27 +1569,27 @@
         <v>41</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>49</v>
       </c>
@@ -1571,7 +1597,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>62</v>
       </c>
@@ -1582,7 +1608,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>38</v>
       </c>
@@ -1590,12 +1616,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>40</v>
       </c>
@@ -1603,27 +1629,27 @@
         <v>41</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>49</v>
       </c>
@@ -1634,7 +1660,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>63</v>
       </c>
@@ -1645,7 +1671,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>38</v>
       </c>
@@ -1653,12 +1679,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>40</v>
       </c>
@@ -1666,27 +1692,27 @@
         <v>41</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>49</v>
       </c>
@@ -1697,7 +1723,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>64</v>
       </c>
@@ -1705,7 +1731,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>38</v>
       </c>
@@ -1713,12 +1739,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B99" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>40</v>
       </c>
@@ -1726,27 +1752,27 @@
         <v>41</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>49</v>
       </c>
@@ -1754,7 +1780,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>66</v>
       </c>
@@ -1762,7 +1788,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>38</v>
       </c>
@@ -1770,12 +1796,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>40</v>
       </c>
@@ -1783,27 +1809,27 @@
         <v>41</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B111" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B112" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B114" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>49</v>
       </c>
@@ -1811,7 +1837,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>68</v>
       </c>
@@ -1819,7 +1845,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>38</v>
       </c>
@@ -1827,12 +1853,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B119" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>40</v>
       </c>
@@ -1840,27 +1866,27 @@
         <v>41</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B121" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B122" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B123" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B124" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
Header, footer, abstract pages
Co-Authored-By: Lorenzo-Guerrieri-98 <56880256+Lorenzo-Guerrieri-98@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Design-part/UX diagram part A1 HYP design in the small and abstract pages.xlsx
+++ b/Design-part/UX diagram part A1 HYP design in the small and abstract pages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carloambrogi/Desktop/Hypermedia-Project/Design-part/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\GitHub\Hypermedia-Project\Design-part\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA747284-1ED0-1345-8856-C614941FF4DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35301736-7DC6-4B08-87D1-998E5EB5DA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{CF35C348-60D3-C34C-B3F9-EC827BB88FFA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{CF35C348-60D3-C34C-B3F9-EC827BB88FFA}"/>
   </bookViews>
   <sheets>
     <sheet name="Content tables" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="84">
   <si>
     <t>Topic: "Town"</t>
   </si>
@@ -197,33 +197,18 @@
     <t>Transition links</t>
   </si>
   <si>
-    <t>Point of interest where hosted</t>
-  </si>
-  <si>
     <t>Page for kind of topic: "Point of interests"</t>
   </si>
   <si>
-    <t>Event hosted</t>
-  </si>
-  <si>
-    <t>Itineraries involving</t>
-  </si>
-  <si>
     <t>Page for kind of topic: "Itineraries"</t>
   </si>
   <si>
-    <t>Included point of interests</t>
-  </si>
-  <si>
     <t>Page for kind of topic: "Services type"</t>
   </si>
   <si>
     <t>Page for group: "All events"</t>
   </si>
   <si>
-    <t>Page for the kind of topic event</t>
-  </si>
-  <si>
     <t>Page for group: "All summer events"</t>
   </si>
   <si>
@@ -233,21 +218,12 @@
     <t>Page for group: "All points of interest"</t>
   </si>
   <si>
-    <t>Page for the kind of topic point of interests</t>
-  </si>
-  <si>
     <t>Page for group: "All itineraries"</t>
   </si>
   <si>
-    <t>Page for the kind of topic itineraries</t>
-  </si>
-  <si>
     <t>Page for group: "All services"</t>
   </si>
   <si>
-    <t>Page for the kind of topic service types</t>
-  </si>
-  <si>
     <t>Column1</t>
   </si>
   <si>
@@ -266,34 +242,52 @@
     <t>All services</t>
   </si>
   <si>
-    <t>All services type</t>
-  </si>
-  <si>
-    <t>? È necessario?</t>
-  </si>
-  <si>
-    <t>Column2</t>
-  </si>
-  <si>
-    <t>?? Breadcrump?</t>
-  </si>
-  <si>
-    <t>? Pagine separate?</t>
-  </si>
-  <si>
-    <t>idem come sopra</t>
-  </si>
-  <si>
-    <t>Colonna1</t>
-  </si>
-  <si>
-    <t>sceglere come rappresentarlo</t>
-  </si>
-  <si>
     <t>Title: Service type name</t>
   </si>
   <si>
-    <t>questo sarà la prewiew per il group link</t>
+    <t>List: name, date, short description (50 words) --&gt; preview of group link</t>
+  </si>
+  <si>
+    <t>List of points of interests: text 50 words for each point --&gt; preview of transition link</t>
+  </si>
+  <si>
+    <t>List: name, image [0:1], short description (50 words) --&gt; preview of group link</t>
+  </si>
+  <si>
+    <t>List: name, duration / length, short description (theme) (50 words) --&gt; preview of group link</t>
+  </si>
+  <si>
+    <t>List: name of the service --&gt; preview of group link</t>
+  </si>
+  <si>
+    <t>Point of interest where hosted (thumbnail + name + short description)</t>
+  </si>
+  <si>
+    <t>Event hosted (thumbnail + name + period (+ short description))</t>
+  </si>
+  <si>
+    <t>Itineraries involving (name + length + duration + short description)</t>
+  </si>
+  <si>
+    <t>Included point of interests (thumbnail + name + short description)</t>
+  </si>
+  <si>
+    <t>All services (i.e., the link above, inside the landmark)</t>
+  </si>
+  <si>
+    <t>Page for the kind of topic event (thumbnail + name + date + short description)</t>
+  </si>
+  <si>
+    <t>Page for the kind of topic event  (thumbnail + name + date + short description)</t>
+  </si>
+  <si>
+    <t>Page for the kind of topic point of interests (thumbnail + short descripion + free/not free)</t>
+  </si>
+  <si>
+    <t>Page for the kind of topic itineraries (thumbnail + name + length/duration + short description)</t>
+  </si>
+  <si>
+    <t>Page for the kind of topic service types (name)</t>
   </si>
 </sst>
 </file>
@@ -339,7 +333,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -396,12 +390,11 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{6DDB3FB5-D071-4A32-885B-8B86FDD5FAC8}" name="Table15" displayName="Table15" ref="A16:C27" totalsRowShown="0">
-  <autoFilter ref="A16:C27" xr:uid="{6DDB3FB5-D071-4A32-885B-8B86FDD5FAC8}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{6DDB3FB5-D071-4A32-885B-8B86FDD5FAC8}" name="Table15" displayName="Table15" ref="A16:B27" totalsRowShown="0">
+  <autoFilter ref="A16:B27" xr:uid="{6DDB3FB5-D071-4A32-885B-8B86FDD5FAC8}"/>
+  <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{CF67C389-C2D4-43D6-94BF-7AF9744F66FC}" name="Page for kind of topic: &quot;Events&quot;"/>
     <tableColumn id="2" xr3:uid="{8DE05ECF-AB8D-417E-BC77-E1ABEBC32636}" name="Column1"/>
-    <tableColumn id="3" xr3:uid="{54EFB7B2-58F8-CB45-982E-CEFA45CD2EFE}" name="Column2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -430,12 +423,11 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{23E1F1C1-7550-483B-857A-D63608F13F1F}" name="Table18" displayName="Table18" ref="A57:C65" totalsRowShown="0">
-  <autoFilter ref="A57:C65" xr:uid="{23E1F1C1-7550-483B-857A-D63608F13F1F}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{23E1F1C1-7550-483B-857A-D63608F13F1F}" name="Table18" displayName="Table18" ref="A57:B65" totalsRowShown="0">
+  <autoFilter ref="A57:B65" xr:uid="{23E1F1C1-7550-483B-857A-D63608F13F1F}"/>
+  <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{D07584D9-1A8F-41AF-A3ED-62DF307BB8E3}" name="Page for kind of topic: &quot;Services type&quot;"/>
     <tableColumn id="2" xr3:uid="{54BDE5B2-8009-46CF-BB76-9E311B842315}" name="Column1"/>
-    <tableColumn id="3" xr3:uid="{B72DEDCA-0947-4AC7-B934-BA3B2CF50199}" name="Column2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -453,24 +445,22 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{950BC4F7-D3EE-499C-93A7-A5E79CEC86F6}" name="Table20" displayName="Table20" ref="A77:C85" totalsRowShown="0">
-  <autoFilter ref="A77:C85" xr:uid="{950BC4F7-D3EE-499C-93A7-A5E79CEC86F6}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{950BC4F7-D3EE-499C-93A7-A5E79CEC86F6}" name="Table20" displayName="Table20" ref="A77:B85" totalsRowShown="0">
+  <autoFilter ref="A77:B85" xr:uid="{950BC4F7-D3EE-499C-93A7-A5E79CEC86F6}"/>
+  <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{995209C7-D184-4899-8288-2AB16102B79C}" name="Page for group: &quot;All summer events&quot;"/>
     <tableColumn id="2" xr3:uid="{175BA796-CDDD-4177-A3C4-AF866FEB34B1}" name="Group &quot;All summer events&quot;"/>
-    <tableColumn id="3" xr3:uid="{DAA39DA6-73BA-43DC-9A28-350EDB0BD579}" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{47676A86-326F-4B55-8642-E1FA72DA0872}" name="Table21" displayName="Table21" ref="A87:C95" totalsRowShown="0">
-  <autoFilter ref="A87:C95" xr:uid="{47676A86-326F-4B55-8642-E1FA72DA0872}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{47676A86-326F-4B55-8642-E1FA72DA0872}" name="Table21" displayName="Table21" ref="A87:B95" totalsRowShown="0">
+  <autoFilter ref="A87:B95" xr:uid="{47676A86-326F-4B55-8642-E1FA72DA0872}"/>
+  <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{9B91B707-C483-46E5-915E-4072C1F8E73F}" name="Page for group: &quot;All winter events&quot;"/>
     <tableColumn id="2" xr3:uid="{C55F7825-FC40-4CE0-9988-4931B60B7D54}" name="Column1"/>
-    <tableColumn id="3" xr3:uid="{CA91B47A-77CB-4AA2-8D05-258F34793573}" name="Column2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -540,11 +530,10 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A66A5AF2-B58F-4EFE-BBF0-A9C7E6F124D6}" name="Table7" displayName="Table7" ref="A27:B29" totalsRowShown="0">
-  <autoFilter ref="A27:B29" xr:uid="{A66A5AF2-B58F-4EFE-BBF0-A9C7E6F124D6}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A66A5AF2-B58F-4EFE-BBF0-A9C7E6F124D6}" name="Table7" displayName="Table7" ref="A27:A29" totalsRowShown="0">
+  <autoFilter ref="A27:A29" xr:uid="{A66A5AF2-B58F-4EFE-BBF0-A9C7E6F124D6}"/>
+  <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{D162CF21-5F29-4B11-9384-455A4BE78ACA}" name="Kind of topic &quot;Services type&quot;"/>
-    <tableColumn id="2" xr3:uid="{C5742220-14CA-574E-A206-CAE6B6D2F1A6}" name="Colonna1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -591,7 +580,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -887,236 +876,230 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7009AE2-141B-8F43-BF6B-7E6ECFF7233C}">
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:A53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="171" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="74.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>17</v>
       </c>
-      <c r="B27" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>19</v>
       </c>
-      <c r="B29" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1139,55 +1122,55 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F52FC61-8669-774A-ACF5-BEF7FABCEB04}">
-  <dimension ref="A1:C125"/>
+  <dimension ref="A1:B125"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" topLeftCell="A118" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="65.1640625" customWidth="1"/>
     <col min="2" max="2" width="62.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -1195,27 +1178,27 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1223,28 +1206,25 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>50</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
-      </c>
-      <c r="C16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -1252,22 +1232,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -1275,27 +1255,27 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>49</v>
       </c>
@@ -1303,26 +1283,23 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>52</v>
       </c>
       <c r="B27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>53</v>
       </c>
-      <c r="C27" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>54</v>
-      </c>
       <c r="B29" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -1330,22 +1307,22 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -1353,27 +1330,27 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>49</v>
       </c>
@@ -1381,28 +1358,28 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>52</v>
       </c>
       <c r="B40" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B43" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>38</v>
       </c>
@@ -1410,27 +1387,27 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>40</v>
       </c>
@@ -1438,27 +1415,27 @@
         <v>41</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>49</v>
       </c>
@@ -1466,39 +1443,36 @@
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>52</v>
       </c>
       <c r="B55" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>70</v>
-      </c>
-      <c r="C57" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>38</v>
       </c>
       <c r="B58" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B59" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>40</v>
       </c>
@@ -1506,49 +1480,43 @@
         <v>41</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
-        <v>75</v>
-      </c>
-      <c r="C64" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>49</v>
       </c>
       <c r="B65" t="s">
-        <v>76</v>
-      </c>
-      <c r="C65" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B67" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>38</v>
       </c>
@@ -1556,12 +1524,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B69" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>40</v>
       </c>
@@ -1569,46 +1537,43 @@
         <v>41</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B71" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B72" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B73" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B74" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>49</v>
       </c>
       <c r="B75" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B77" t="s">
         <v>23</v>
       </c>
-      <c r="C77" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>38</v>
       </c>
@@ -1616,12 +1581,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B79" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>40</v>
       </c>
@@ -1629,49 +1594,43 @@
         <v>41</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B81" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B82" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B83" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B84" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>49</v>
       </c>
       <c r="B85" t="s">
-        <v>61</v>
-      </c>
-      <c r="C85" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B87" t="s">
-        <v>70</v>
-      </c>
-      <c r="C87" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>38</v>
       </c>
@@ -1679,12 +1638,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B89" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>40</v>
       </c>
@@ -1692,46 +1651,43 @@
         <v>41</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B91" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B92" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B93" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B94" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>49</v>
       </c>
       <c r="B95" t="s">
-        <v>61</v>
-      </c>
-      <c r="C95" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B97" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>38</v>
       </c>
@@ -1739,12 +1695,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B99" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>40</v>
       </c>
@@ -1752,43 +1708,43 @@
         <v>41</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B101" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B102" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B103" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B104" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>49</v>
       </c>
       <c r="B105" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B107" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>38</v>
       </c>
@@ -1796,12 +1752,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B109" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>40</v>
       </c>
@@ -1809,43 +1765,43 @@
         <v>41</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B111" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B112" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B113" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B114" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>49</v>
       </c>
       <c r="B115" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B117" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>38</v>
       </c>
@@ -1853,12 +1809,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B119" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>40</v>
       </c>
@@ -1866,32 +1822,32 @@
         <v>41</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B121" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B122" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B123" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B124" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>49</v>
       </c>
       <c r="B125" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Prototype for POI card
</commit_message>
<xml_diff>
--- a/Design-part/UX diagram part A1 HYP design in the small and abstract pages.xlsx
+++ b/Design-part/UX diagram part A1 HYP design in the small and abstract pages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\GitHub\Hypermedia-Project\Design-part\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35301736-7DC6-4B08-87D1-998E5EB5DA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD151CF-DAC4-435A-9541-B512EA46197B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{CF35C348-60D3-C34C-B3F9-EC827BB88FFA}"/>
   </bookViews>
@@ -1124,8 +1124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F52FC61-8669-774A-ACF5-BEF7FABCEB04}">
   <dimension ref="A1:B125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Started to do itineraries
</commit_message>
<xml_diff>
--- a/Design-part/UX diagram part A1 HYP design in the small and abstract pages.xlsx
+++ b/Design-part/UX diagram part A1 HYP design in the small and abstract pages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\GitHub\Hypermedia-Project\Design-part\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carloambrogi/Desktop/Hypermedia-Project/Design-part/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35301736-7DC6-4B08-87D1-998E5EB5DA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78C8FCA-B7B4-9A4E-8C46-604AC00919CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{CF35C348-60D3-C34C-B3F9-EC827BB88FFA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" activeTab="1" xr2:uid="{CF35C348-60D3-C34C-B3F9-EC827BB88FFA}"/>
   </bookViews>
   <sheets>
     <sheet name="Content tables" sheetId="1" r:id="rId1"/>
@@ -284,10 +284,10 @@
     <t>Page for the kind of topic point of interests (thumbnail + short descripion + free/not free)</t>
   </si>
   <si>
-    <t>Page for the kind of topic itineraries (thumbnail + name + length/duration + short description)</t>
-  </si>
-  <si>
     <t>Page for the kind of topic service types (name)</t>
+  </si>
+  <si>
+    <t>Page for the kind of topic itineraries (name + length/duration + short description)</t>
   </si>
 </sst>
 </file>
@@ -333,7 +333,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -580,7 +580,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -882,222 +882,222 @@
       <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="74.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>73</v>
       </c>
@@ -1124,17 +1124,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F52FC61-8669-774A-ACF5-BEF7FABCEB04}">
   <dimension ref="A1:B125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A92" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D114" sqref="D114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="65.1640625" customWidth="1"/>
     <col min="2" max="2" width="62.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -1150,27 +1150,27 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -1178,27 +1178,27 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1206,17 +1206,17 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -1232,22 +1232,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -1255,27 +1255,27 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>49</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -1299,7 +1299,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -1307,22 +1307,22 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -1330,27 +1330,27 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>49</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -1366,12 +1366,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>54</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>38</v>
       </c>
@@ -1387,27 +1387,27 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>40</v>
       </c>
@@ -1415,27 +1415,27 @@
         <v>41</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>49</v>
       </c>
@@ -1443,7 +1443,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>52</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>38</v>
       </c>
@@ -1467,12 +1467,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>40</v>
       </c>
@@ -1480,27 +1480,27 @@
         <v>41</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>49</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>56</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>38</v>
       </c>
@@ -1524,12 +1524,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>40</v>
       </c>
@@ -1537,27 +1537,27 @@
         <v>41</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>49</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>57</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>38</v>
       </c>
@@ -1581,12 +1581,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>40</v>
       </c>
@@ -1594,27 +1594,27 @@
         <v>41</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>49</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>58</v>
       </c>
@@ -1630,7 +1630,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>38</v>
       </c>
@@ -1638,12 +1638,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>40</v>
       </c>
@@ -1651,27 +1651,27 @@
         <v>41</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>49</v>
       </c>
@@ -1679,7 +1679,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>59</v>
       </c>
@@ -1687,7 +1687,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>38</v>
       </c>
@@ -1695,12 +1695,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B99" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>40</v>
       </c>
@@ -1708,27 +1708,27 @@
         <v>41</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>49</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>60</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>38</v>
       </c>
@@ -1752,12 +1752,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>40</v>
       </c>
@@ -1765,35 +1765,35 @@
         <v>41</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B111" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B112" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B114" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>49</v>
       </c>
       <c r="B115" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>61</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>38</v>
       </c>
@@ -1809,12 +1809,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B119" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>40</v>
       </c>
@@ -1822,32 +1822,32 @@
         <v>41</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B121" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B122" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B123" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B124" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>49</v>
       </c>
       <c r="B125" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Footer; Contact us (page, excel, low wireframe)
</commit_message>
<xml_diff>
--- a/Design-part/UX diagram part A1 HYP design in the small and abstract pages.xlsx
+++ b/Design-part/UX diagram part A1 HYP design in the small and abstract pages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carloambrogi/Desktop/Hypermedia-Project/Design-part/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4CFEAC3-45EA-9048-89A4-8A651842F961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A1FB7E-83C5-4A4C-A239-C28B044F555D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" activeTab="1" xr2:uid="{CF35C348-60D3-C34C-B3F9-EC827BB88FFA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="89">
   <si>
     <t>Kind of topic "Events"</t>
   </si>
@@ -288,13 +288,28 @@
   </si>
   <si>
     <t>Page for the kind of topic itineraries (thumbnail, name, duration, length, short description)</t>
+  </si>
+  <si>
+    <t>Page for topic: "Contact us"</t>
+  </si>
+  <si>
+    <t>Title: "VisitMantova"</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Topic: "Contact us"</t>
+  </si>
+  <si>
+    <t>Contact us</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -309,8 +324,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -323,8 +346,20 @@
         <bgColor rgb="FFD9E1F2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -347,14 +382,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -383,8 +449,8 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D6480563-9F9D-4FF1-8AAB-5F2815E4C67A}" name="Table12" displayName="Table12" ref="A63:A65" totalsRowShown="0">
-  <autoFilter ref="A63:A65" xr:uid="{D6480563-9F9D-4FF1-8AAB-5F2815E4C67A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D6480563-9F9D-4FF1-8AAB-5F2815E4C67A}" name="Table12" displayName="Table12" ref="A67:A69" totalsRowShown="0">
+  <autoFilter ref="A67:A69" xr:uid="{D6480563-9F9D-4FF1-8AAB-5F2815E4C67A}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{0DD91441-9253-41B6-BC38-1348B60EDB0A}" name="Group &quot;All itineraries&quot;"/>
   </tableColumns>
@@ -393,8 +459,8 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{C54BFB31-5572-45E2-8242-58D85ED38307}" name="Table13" displayName="Table13" ref="A67:A69" totalsRowShown="0">
-  <autoFilter ref="A67:A69" xr:uid="{C54BFB31-5572-45E2-8242-58D85ED38307}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{C54BFB31-5572-45E2-8242-58D85ED38307}" name="Table13" displayName="Table13" ref="A71:A73" totalsRowShown="0">
+  <autoFilter ref="A71:A73" xr:uid="{C54BFB31-5572-45E2-8242-58D85ED38307}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{193BFC96-47DE-4D7A-95BE-7F100BEF7DEB}" name="Group &quot;All services&quot;"/>
   </tableColumns>
@@ -413,8 +479,8 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5CDD5A97-8249-F046-968A-6E67F2D5CA3F}" name="Table145" displayName="Table145" ref="A1:B18" totalsRowShown="0">
-  <autoFilter ref="A1:B18" xr:uid="{8702C592-F3D2-4381-83F1-50BC3271ACBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5CDD5A97-8249-F046-968A-6E67F2D5CA3F}" name="Table145" displayName="Table145" ref="A1:B19" totalsRowShown="0">
+  <autoFilter ref="A1:B19" xr:uid="{8702C592-F3D2-4381-83F1-50BC3271ACBD}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{6F8F84B1-510C-E443-859F-E8E9FCF8DAB0}" name="Page for topic: &quot;Home&quot;"/>
     <tableColumn id="2" xr3:uid="{006DE391-48A3-7B47-A972-85818BDDB5D2}" name="Column1"/>
@@ -424,8 +490,8 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{EA050A5E-7CD5-FA41-90CE-F083B75F5BFC}" name="Table1526" displayName="Table1526" ref="A38:B52" totalsRowShown="0">
-  <autoFilter ref="A38:B52" xr:uid="{6DDB3FB5-D071-4A32-885B-8B86FDD5FAC8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{EA050A5E-7CD5-FA41-90CE-F083B75F5BFC}" name="Table1526" displayName="Table1526" ref="A40:B55" totalsRowShown="0">
+  <autoFilter ref="A40:B55" xr:uid="{6DDB3FB5-D071-4A32-885B-8B86FDD5FAC8}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{D234D3EF-8EEC-054C-9818-75531F360673}" name="Page for kind of topic: &quot;Events&quot;"/>
     <tableColumn id="2" xr3:uid="{8F37BBC1-A658-7744-AA8B-870155E12982}" name="Column1"/>
@@ -435,8 +501,8 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{98DA46B7-F592-FD40-A205-AD02F764F65B}" name="Table1627" displayName="Table1627" ref="A54:B68" totalsRowShown="0">
-  <autoFilter ref="A54:B68" xr:uid="{69973426-9D98-4C80-B65C-9CEC0CA019B5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{98DA46B7-F592-FD40-A205-AD02F764F65B}" name="Table1627" displayName="Table1627" ref="A57:B72" totalsRowShown="0">
+  <autoFilter ref="A57:B72" xr:uid="{69973426-9D98-4C80-B65C-9CEC0CA019B5}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{F38CF9EC-BF8E-BF4A-A35C-D4F3FB1B4AD0}" name="Page for kind of topic: &quot;Point of interests&quot;"/>
     <tableColumn id="2" xr3:uid="{EB3A77A6-77E3-A548-B6B2-D60ACDD359F0}" name="Column1"/>
@@ -446,8 +512,8 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="27" xr:uid="{385354CF-4CEB-094F-86E8-F1ACF3B10B76}" name="Table1728" displayName="Table1728" ref="A70:B84" totalsRowShown="0">
-  <autoFilter ref="A70:B84" xr:uid="{E633F259-7F64-4708-8917-88CB681107AF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="27" xr:uid="{385354CF-4CEB-094F-86E8-F1ACF3B10B76}" name="Table1728" displayName="Table1728" ref="A74:B89" totalsRowShown="0">
+  <autoFilter ref="A74:B89" xr:uid="{E633F259-7F64-4708-8917-88CB681107AF}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{7384952C-6E37-5248-A562-1BDD1547BA7F}" name="Page for kind of topic: &quot;Itineraries&quot;"/>
     <tableColumn id="2" xr3:uid="{B5EC250A-4445-4343-B207-16515496A925}" name="Column1"/>
@@ -457,8 +523,8 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="28" xr:uid="{BD044C5E-0E04-9645-82AD-333BE7591A12}" name="Table1829" displayName="Table1829" ref="A86:B96" totalsRowShown="0">
-  <autoFilter ref="A86:B96" xr:uid="{23E1F1C1-7550-483B-857A-D63608F13F1F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="28" xr:uid="{BD044C5E-0E04-9645-82AD-333BE7591A12}" name="Table1829" displayName="Table1829" ref="A91:B102" totalsRowShown="0">
+  <autoFilter ref="A91:B102" xr:uid="{23E1F1C1-7550-483B-857A-D63608F13F1F}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{8BCFEA6C-EF7B-F24E-A5F9-5C58A84A2699}" name="Page for kind of topic: &quot;Services type&quot;"/>
     <tableColumn id="2" xr3:uid="{42EFE230-4FFA-5940-821C-5A94CB0EDEF5}" name="Column1"/>
@@ -468,8 +534,8 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="29" xr:uid="{55FEF2F9-6341-C247-9487-CFEFD17FCE16}" name="Table1930" displayName="Table1930" ref="A98:B109" totalsRowShown="0">
-  <autoFilter ref="A98:B109" xr:uid="{E3E927A6-B68F-4E61-A3D7-F69689C11112}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="29" xr:uid="{55FEF2F9-6341-C247-9487-CFEFD17FCE16}" name="Table1930" displayName="Table1930" ref="A116:B128" totalsRowShown="0">
+  <autoFilter ref="A116:B128" xr:uid="{E3E927A6-B68F-4E61-A3D7-F69689C11112}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{8D4B2448-8015-7C45-B908-ED9EC8D412BA}" name="Page for group: &quot;All events&quot;"/>
     <tableColumn id="2" xr3:uid="{7FC86B2C-B2EA-5B45-8407-382B9ECCC1D8}" name="Column1"/>
@@ -479,8 +545,8 @@
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="30" xr:uid="{A227AA2E-5D6D-0348-A268-39F0C01F1493}" name="Table2031" displayName="Table2031" ref="A111:B122" totalsRowShown="0">
-  <autoFilter ref="A111:B122" xr:uid="{950BC4F7-D3EE-499C-93A7-A5E79CEC86F6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="30" xr:uid="{A227AA2E-5D6D-0348-A268-39F0C01F1493}" name="Table2031" displayName="Table2031" ref="A130:B142" totalsRowShown="0">
+  <autoFilter ref="A130:B142" xr:uid="{950BC4F7-D3EE-499C-93A7-A5E79CEC86F6}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{361A93E6-9656-B14D-8C82-3BA6F871E2A9}" name="Page for group: &quot;All summer events&quot;"/>
     <tableColumn id="2" xr3:uid="{8AD30F5A-AC89-2D46-B527-A99E6E56A427}" name="Group &quot;All summer events&quot;"/>
@@ -490,8 +556,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F8792E6E-3B14-44D0-8477-FFA7441AA628}" name="Table3" displayName="Table3" ref="A24:A28" totalsRowShown="0">
-  <autoFilter ref="A24:A28" xr:uid="{F8792E6E-3B14-44D0-8477-FFA7441AA628}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F8792E6E-3B14-44D0-8477-FFA7441AA628}" name="Table3" displayName="Table3" ref="A28:A32" totalsRowShown="0">
+  <autoFilter ref="A28:A32" xr:uid="{F8792E6E-3B14-44D0-8477-FFA7441AA628}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{9AC80452-1CDF-458E-A69F-D516DDBCDF7C}" name="Kind of topic &quot;Events&quot;"/>
   </tableColumns>
@@ -500,8 +566,8 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="31" xr:uid="{31713721-7F1E-9B40-9FAD-E5E0012F8CED}" name="Table2132" displayName="Table2132" ref="A124:B135" totalsRowShown="0">
-  <autoFilter ref="A124:B135" xr:uid="{47676A86-326F-4B55-8642-E1FA72DA0872}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="31" xr:uid="{31713721-7F1E-9B40-9FAD-E5E0012F8CED}" name="Table2132" displayName="Table2132" ref="A144:B156" totalsRowShown="0">
+  <autoFilter ref="A144:B156" xr:uid="{47676A86-326F-4B55-8642-E1FA72DA0872}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{40C615F9-7C3C-4F42-9F21-D9DDC9A72D6C}" name="Page for group: &quot;All winter events&quot;"/>
     <tableColumn id="2" xr3:uid="{D8ED8285-E648-1047-87D8-C3D5B6509C40}" name="Column1"/>
@@ -511,8 +577,8 @@
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="32" xr:uid="{A59002C8-F1F5-D94D-8B5A-66A9B06738AD}" name="Table2233" displayName="Table2233" ref="A137:B148" totalsRowShown="0">
-  <autoFilter ref="A137:B148" xr:uid="{ECF51F54-57EE-4277-8583-FC66BDE82BDE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="32" xr:uid="{A59002C8-F1F5-D94D-8B5A-66A9B06738AD}" name="Table2233" displayName="Table2233" ref="A158:B170" totalsRowShown="0">
+  <autoFilter ref="A158:B170" xr:uid="{ECF51F54-57EE-4277-8583-FC66BDE82BDE}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{FDBDC38E-C29F-C842-B0DF-BB9B4B41D86F}" name="Page for group: &quot;All points of interest&quot;"/>
     <tableColumn id="2" xr3:uid="{72470908-B945-E84A-B193-8B89B43D779D}" name="Column1"/>
@@ -522,8 +588,8 @@
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="33" xr:uid="{6B5CE5B3-EAE2-1C4E-BE3B-15B4434A7026}" name="Table2334" displayName="Table2334" ref="A150:B161" totalsRowShown="0">
-  <autoFilter ref="A150:B161" xr:uid="{17C4130F-4729-47ED-AFA7-C61CB4A33D00}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="33" xr:uid="{6B5CE5B3-EAE2-1C4E-BE3B-15B4434A7026}" name="Table2334" displayName="Table2334" ref="A172:B184" totalsRowShown="0">
+  <autoFilter ref="A172:B184" xr:uid="{17C4130F-4729-47ED-AFA7-C61CB4A33D00}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{A7644BBC-B281-C540-B1BF-0263A28CA359}" name="Page for group: &quot;All itineraries&quot;"/>
     <tableColumn id="2" xr3:uid="{A9C9CFE3-BF94-2E40-87D4-7C6DA54F1773}" name="Column1"/>
@@ -533,8 +599,8 @@
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{AD6838DD-4E69-3546-81FC-9C63610B1F7F}" name="Table2435" displayName="Table2435" ref="A163:B174" totalsRowShown="0">
-  <autoFilter ref="A163:B174" xr:uid="{4421B5D6-37B1-43A6-8C29-3894C8A06CEF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{AD6838DD-4E69-3546-81FC-9C63610B1F7F}" name="Table2435" displayName="Table2435" ref="A186:B198" totalsRowShown="0">
+  <autoFilter ref="A186:B198" xr:uid="{4421B5D6-37B1-43A6-8C29-3894C8A06CEF}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{1A2F8E68-4BDB-3B4A-8BDB-A1F6774D7E76}" name="Page for group: &quot;All services&quot;"/>
     <tableColumn id="2" xr3:uid="{47486761-2689-114D-9EB5-567D69EF092D}" name="Column1"/>
@@ -544,8 +610,8 @@
 </file>
 
 <file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="35" xr:uid="{2BBC3333-1425-364C-913D-4BB8B278199E}" name="Table14536" displayName="Table14536" ref="A20:B36" totalsRowShown="0">
-  <autoFilter ref="A20:B36" xr:uid="{2BBC3333-1425-364C-913D-4BB8B278199E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="35" xr:uid="{2BBC3333-1425-364C-913D-4BB8B278199E}" name="Table14536" displayName="Table14536" ref="A21:B38" totalsRowShown="0">
+  <autoFilter ref="A21:B38" xr:uid="{2BBC3333-1425-364C-913D-4BB8B278199E}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{3D9C43BB-7EEB-0B46-B7F0-7E479ADE26EE}" name="Page for topic: &quot;About&quot;"/>
     <tableColumn id="2" xr3:uid="{4F4091F0-FC12-1C40-9A35-1FCF58C7E7D3}" name="Column1"/>
@@ -554,9 +620,20 @@
 </table>
 </file>
 
+<file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{64F84DE1-EB04-AF46-B69F-E4C9D4E8E83C}" name="Table1453615" displayName="Table1453615" ref="A104:B114" totalsRowShown="0">
+  <autoFilter ref="A104:B114" xr:uid="{64F84DE1-EB04-AF46-B69F-E4C9D4E8E83C}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{ABE14190-B15A-BE4A-8325-00A1F15143DB}" name="Page for topic: &quot;Contact us&quot;"/>
+    <tableColumn id="2" xr3:uid="{6EF1ECF7-38B6-6C49-8992-176DB81725CA}" name="Column1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0EF7AB7F-0B91-4374-BFD8-CB0CB79FF7FF}" name="Table5" displayName="Table5" ref="A30:A34" totalsRowShown="0">
-  <autoFilter ref="A30:A34" xr:uid="{0EF7AB7F-0B91-4374-BFD8-CB0CB79FF7FF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0EF7AB7F-0B91-4374-BFD8-CB0CB79FF7FF}" name="Table5" displayName="Table5" ref="A34:A38" totalsRowShown="0">
+  <autoFilter ref="A34:A38" xr:uid="{0EF7AB7F-0B91-4374-BFD8-CB0CB79FF7FF}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{74D0489E-FA72-48A7-AD1F-AAE7E005328E}" name="Kind of topic &quot;Point of interests&quot;"/>
   </tableColumns>
@@ -565,8 +642,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{0F2C3591-F6A8-4CE0-8142-AD74C0A61324}" name="Table6" displayName="Table6" ref="A36:A41" totalsRowShown="0">
-  <autoFilter ref="A36:A41" xr:uid="{0F2C3591-F6A8-4CE0-8142-AD74C0A61324}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{0F2C3591-F6A8-4CE0-8142-AD74C0A61324}" name="Table6" displayName="Table6" ref="A40:A45" totalsRowShown="0">
+  <autoFilter ref="A40:A45" xr:uid="{0F2C3591-F6A8-4CE0-8142-AD74C0A61324}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{60918BAD-E74B-4272-B1D1-6A938ABA4CD9}" name="Kind of topic &quot;Itineraries&quot;"/>
   </tableColumns>
@@ -575,8 +652,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A66A5AF2-B58F-4EFE-BBF0-A9C7E6F124D6}" name="Table7" displayName="Table7" ref="A43:A45" totalsRowShown="0">
-  <autoFilter ref="A43:A45" xr:uid="{A66A5AF2-B58F-4EFE-BBF0-A9C7E6F124D6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A66A5AF2-B58F-4EFE-BBF0-A9C7E6F124D6}" name="Table7" displayName="Table7" ref="A47:A49" totalsRowShown="0">
+  <autoFilter ref="A47:A49" xr:uid="{A66A5AF2-B58F-4EFE-BBF0-A9C7E6F124D6}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{D162CF21-5F29-4B11-9384-455A4BE78ACA}" name="Kind of topic &quot;Services type&quot;"/>
   </tableColumns>
@@ -585,8 +662,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{48C80BC2-F23E-406B-8F6F-31D91E717C56}" name="Table8" displayName="Table8" ref="A47:A49" totalsRowShown="0">
-  <autoFilter ref="A47:A49" xr:uid="{48C80BC2-F23E-406B-8F6F-31D91E717C56}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{48C80BC2-F23E-406B-8F6F-31D91E717C56}" name="Table8" displayName="Table8" ref="A51:A53" totalsRowShown="0">
+  <autoFilter ref="A51:A53" xr:uid="{48C80BC2-F23E-406B-8F6F-31D91E717C56}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{26497DED-FBCE-4947-B3EB-C2BF72444227}" name="Group &quot;All events&quot;"/>
   </tableColumns>
@@ -595,8 +672,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{46480F79-8355-403B-AC23-B1D3DE68F15C}" name="Table9" displayName="Table9" ref="A51:A53" totalsRowShown="0">
-  <autoFilter ref="A51:A53" xr:uid="{46480F79-8355-403B-AC23-B1D3DE68F15C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{46480F79-8355-403B-AC23-B1D3DE68F15C}" name="Table9" displayName="Table9" ref="A55:A57" totalsRowShown="0">
+  <autoFilter ref="A55:A57" xr:uid="{46480F79-8355-403B-AC23-B1D3DE68F15C}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{2E7831E6-2FE3-42C3-85D0-2246738F6505}" name="Group &quot;All summer events&quot;"/>
   </tableColumns>
@@ -605,8 +682,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{0D3EF7A2-D6B5-4C89-A725-3482A86896F2}" name="Table10" displayName="Table10" ref="A55:A57" totalsRowShown="0">
-  <autoFilter ref="A55:A57" xr:uid="{0D3EF7A2-D6B5-4C89-A725-3482A86896F2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{0D3EF7A2-D6B5-4C89-A725-3482A86896F2}" name="Table10" displayName="Table10" ref="A59:A61" totalsRowShown="0">
+  <autoFilter ref="A59:A61" xr:uid="{0D3EF7A2-D6B5-4C89-A725-3482A86896F2}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{FDF51731-3D09-4129-A59F-C927A9DF0297}" name="Group &quot;All winter events&quot;"/>
   </tableColumns>
@@ -615,8 +692,8 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{49C217C0-4304-4EC7-A582-CE1C2B4D6DB0}" name="Table11" displayName="Table11" ref="A59:A61" totalsRowShown="0">
-  <autoFilter ref="A59:A61" xr:uid="{49C217C0-4304-4EC7-A582-CE1C2B4D6DB0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{49C217C0-4304-4EC7-A582-CE1C2B4D6DB0}" name="Table11" displayName="Table11" ref="A63:A65" totalsRowShown="0">
+  <autoFilter ref="A63:A65" xr:uid="{49C217C0-4304-4EC7-A582-CE1C2B4D6DB0}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{A240D935-E52E-44A0-958C-CE8E64ED8CDC}" name="Group &quot;All points of interest&quot;"/>
   </tableColumns>
@@ -921,10 +998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7009AE2-141B-8F43-BF6B-7E6ECFF7233C}">
-  <dimension ref="A1:A69"/>
+  <dimension ref="A1:A73"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
+    <sheetView topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1038,123 +1115,123 @@
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>0</v>
+      <c r="A24" s="5" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>1</v>
+      <c r="A25" s="3" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>2</v>
+      <c r="A26" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>5</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>3</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>79</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>80</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>10</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
@@ -1164,12 +1241,12 @@
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
@@ -1179,46 +1256,61 @@
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1243,10 +1335,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D009084-A617-FE43-A7BE-1BA4673EB7A1}">
-  <dimension ref="A1:B174"/>
+  <dimension ref="A1:B198"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1350,903 +1442,1033 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>24</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>73</v>
-      </c>
-      <c r="B20" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>23</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>75</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>68</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>77</v>
-      </c>
-      <c r="B36" t="s">
-        <v>76</v>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>28</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>23</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B41" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B40" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>75</v>
-      </c>
       <c r="B43" t="s">
-        <v>67</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>75</v>
+      </c>
       <c r="B45" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>69</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>77</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B53" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>27</v>
-      </c>
-      <c r="B51" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>29</v>
-      </c>
-      <c r="B52" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B54" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>29</v>
+      </c>
+      <c r="B55" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>30</v>
+      </c>
+      <c r="B57" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>23</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B58" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B56" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B57" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B58" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>75</v>
-      </c>
-      <c r="B59" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>68</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>75</v>
+      </c>
       <c r="B62" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
-        <v>70</v>
+        <v>26</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>77</v>
-      </c>
       <c r="B66" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>29</v>
-      </c>
       <c r="B67" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
-        <v>43</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B69" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>31</v>
+        <v>77</v>
       </c>
       <c r="B70" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B71" t="s">
-        <v>7</v>
+        <v>78</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>31</v>
+      </c>
+      <c r="B74" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>23</v>
+      </c>
+      <c r="B75" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B76" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B73" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B74" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B75" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>75</v>
-      </c>
-      <c r="B76" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>75</v>
+      </c>
       <c r="B80" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B83" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B84" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B85" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B86" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B87" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
         <v>77</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B88" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>29</v>
-      </c>
-      <c r="B84" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>32</v>
-      </c>
-      <c r="B86" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>23</v>
-      </c>
-      <c r="B87" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B88" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>75</v>
+        <v>29</v>
       </c>
       <c r="B89" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B90" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>32</v>
+      </c>
       <c r="B91" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>23</v>
+      </c>
       <c r="B92" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>75</v>
+      </c>
       <c r="B94" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
-        <v>77</v>
-      </c>
       <c r="B96" t="s">
-        <v>76</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B97" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
-        <v>33</v>
-      </c>
       <c r="B98" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
-        <v>23</v>
-      </c>
       <c r="B99" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
-        <v>75</v>
-      </c>
       <c r="B101" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>77</v>
+      </c>
       <c r="B102" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B103" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>84</v>
+      </c>
       <c r="B104" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>23</v>
+      </c>
       <c r="B105" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B106" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>75</v>
+      </c>
       <c r="B107" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
-        <v>77</v>
-      </c>
       <c r="B108" t="s">
-        <v>76</v>
+        <v>26</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>27</v>
+        <v>86</v>
       </c>
       <c r="B109" t="s">
-        <v>45</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B110" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
-        <v>34</v>
-      </c>
       <c r="B111" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112" t="s">
-        <v>23</v>
-      </c>
       <c r="B112" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B114" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B115" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>33</v>
+      </c>
       <c r="B116" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>23</v>
+      </c>
       <c r="B117" t="s">
-        <v>69</v>
+        <v>12</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B118" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>75</v>
+      </c>
       <c r="B119" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B120" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B121" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B122" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B123" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B124" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B125" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A121" t="s">
-        <v>77</v>
-      </c>
-      <c r="B121" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A122" t="s">
-        <v>27</v>
-      </c>
-      <c r="B122" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A124" t="s">
-        <v>35</v>
-      </c>
-      <c r="B124" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A125" t="s">
-        <v>23</v>
-      </c>
-      <c r="B125" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B126" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B127" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>27</v>
+      </c>
       <c r="B128" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B129" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>34</v>
+      </c>
       <c r="B130" t="s">
-        <v>69</v>
+        <v>13</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>23</v>
+      </c>
       <c r="B131" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B132" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>75</v>
+      </c>
+      <c r="B133" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B134" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B135" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B136" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B137" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B138" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B133" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A134" t="s">
-        <v>77</v>
-      </c>
-      <c r="B134" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A135" t="s">
-        <v>27</v>
-      </c>
-      <c r="B135" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A137" t="s">
-        <v>36</v>
-      </c>
-      <c r="B137" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A138" t="s">
-        <v>23</v>
-      </c>
-      <c r="B138" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B139" t="s">
-        <v>64</v>
+        <v>25</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A140" t="s">
-        <v>75</v>
-      </c>
       <c r="B140" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>77</v>
+      </c>
       <c r="B141" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>27</v>
+      </c>
       <c r="B142" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B143" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>35</v>
+      </c>
       <c r="B144" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>23</v>
+      </c>
       <c r="B145" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B146" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B147" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A148" t="s">
-        <v>27</v>
-      </c>
       <c r="B148" t="s">
-        <v>82</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B149" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A150" t="s">
-        <v>37</v>
-      </c>
       <c r="B150" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A151" t="s">
-        <v>23</v>
-      </c>
       <c r="B151" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B152" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A153" t="s">
-        <v>75</v>
-      </c>
       <c r="B153" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B154" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>77</v>
+      </c>
       <c r="B155" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>27</v>
+      </c>
       <c r="B156" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B157" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>36</v>
+      </c>
       <c r="B158" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>23</v>
+      </c>
       <c r="B159" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A160" t="s">
-        <v>77</v>
-      </c>
       <c r="B160" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="B161" t="s">
-        <v>83</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B162" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A163" t="s">
-        <v>38</v>
-      </c>
       <c r="B163" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A164" t="s">
-        <v>23</v>
-      </c>
       <c r="B164" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B165" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A166" t="s">
-        <v>75</v>
-      </c>
       <c r="B166" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B167" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B168" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>77</v>
+      </c>
       <c r="B169" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>27</v>
+      </c>
       <c r="B170" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B171" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>37</v>
+      </c>
       <c r="B172" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
+        <v>23</v>
+      </c>
+      <c r="B173" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B174" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>75</v>
+      </c>
+      <c r="B175" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B176" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B177" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B178" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B179" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B180" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B181" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B182" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
         <v>77</v>
       </c>
-      <c r="B173" t="s">
+      <c r="B183" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A174" t="s">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
         <v>27</v>
       </c>
-      <c r="B174" t="s">
+      <c r="B184" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>38</v>
+      </c>
+      <c r="B186" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>23</v>
+      </c>
+      <c r="B187" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B188" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>75</v>
+      </c>
+      <c r="B189" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B190" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B191" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B192" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B193" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B194" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B195" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B196" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>77</v>
+      </c>
+      <c r="B197" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>27</v>
+      </c>
+      <c r="B198" t="s">
         <v>47</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="12">
+  <tableParts count="13">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
@@ -2259,6 +2481,7 @@
     <tablePart r:id="rId10"/>
     <tablePart r:id="rId11"/>
     <tablePart r:id="rId12"/>
+    <tablePart r:id="rId13"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the excel (winter summer events)
</commit_message>
<xml_diff>
--- a/Design-part/UX diagram part A1 HYP design in the small and abstract pages.xlsx
+++ b/Design-part/UX diagram part A1 HYP design in the small and abstract pages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carloambrogi/Desktop/Hypermedia-Project/Design-part/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A1FB7E-83C5-4A4C-A239-C28B044F555D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A923AE46-E3CB-924F-A21E-6EB9C813FF4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" activeTab="1" xr2:uid="{CF35C348-60D3-C34C-B3F9-EC827BB88FFA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{CF35C348-60D3-C34C-B3F9-EC827BB88FFA}"/>
   </bookViews>
   <sheets>
     <sheet name="Content tables" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="92">
   <si>
     <t>Kind of topic "Events"</t>
   </si>
@@ -116,9 +116,6 @@
     <t>All service</t>
   </si>
   <si>
-    <t>Events (all, winter, summer)</t>
-  </si>
-  <si>
     <t>Group link</t>
   </si>
   <si>
@@ -303,6 +300,18 @@
   </si>
   <si>
     <t>Contact us</t>
+  </si>
+  <si>
+    <t>Structural links</t>
+  </si>
+  <si>
+    <t>Summer events</t>
+  </si>
+  <si>
+    <t>Winter events</t>
+  </si>
+  <si>
+    <t>Events</t>
   </si>
 </sst>
 </file>
@@ -534,8 +543,8 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="29" xr:uid="{55FEF2F9-6341-C247-9487-CFEFD17FCE16}" name="Table1930" displayName="Table1930" ref="A116:B128" totalsRowShown="0">
-  <autoFilter ref="A116:B128" xr:uid="{E3E927A6-B68F-4E61-A3D7-F69689C11112}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="29" xr:uid="{55FEF2F9-6341-C247-9487-CFEFD17FCE16}" name="Table1930" displayName="Table1930" ref="A116:B130" totalsRowShown="0">
+  <autoFilter ref="A116:B130" xr:uid="{E3E927A6-B68F-4E61-A3D7-F69689C11112}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{8D4B2448-8015-7C45-B908-ED9EC8D412BA}" name="Page for group: &quot;All events&quot;"/>
     <tableColumn id="2" xr3:uid="{7FC86B2C-B2EA-5B45-8407-382B9ECCC1D8}" name="Column1"/>
@@ -545,8 +554,8 @@
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="30" xr:uid="{A227AA2E-5D6D-0348-A268-39F0C01F1493}" name="Table2031" displayName="Table2031" ref="A130:B142" totalsRowShown="0">
-  <autoFilter ref="A130:B142" xr:uid="{950BC4F7-D3EE-499C-93A7-A5E79CEC86F6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="30" xr:uid="{A227AA2E-5D6D-0348-A268-39F0C01F1493}" name="Table2031" displayName="Table2031" ref="A132:B144" totalsRowShown="0">
+  <autoFilter ref="A132:B144" xr:uid="{950BC4F7-D3EE-499C-93A7-A5E79CEC86F6}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{361A93E6-9656-B14D-8C82-3BA6F871E2A9}" name="Page for group: &quot;All summer events&quot;"/>
     <tableColumn id="2" xr3:uid="{8AD30F5A-AC89-2D46-B527-A99E6E56A427}" name="Group &quot;All summer events&quot;"/>
@@ -566,8 +575,8 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="31" xr:uid="{31713721-7F1E-9B40-9FAD-E5E0012F8CED}" name="Table2132" displayName="Table2132" ref="A144:B156" totalsRowShown="0">
-  <autoFilter ref="A144:B156" xr:uid="{47676A86-326F-4B55-8642-E1FA72DA0872}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="31" xr:uid="{31713721-7F1E-9B40-9FAD-E5E0012F8CED}" name="Table2132" displayName="Table2132" ref="A146:B158" totalsRowShown="0">
+  <autoFilter ref="A146:B158" xr:uid="{47676A86-326F-4B55-8642-E1FA72DA0872}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{40C615F9-7C3C-4F42-9F21-D9DDC9A72D6C}" name="Page for group: &quot;All winter events&quot;"/>
     <tableColumn id="2" xr3:uid="{D8ED8285-E648-1047-87D8-C3D5B6509C40}" name="Column1"/>
@@ -577,8 +586,8 @@
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="32" xr:uid="{A59002C8-F1F5-D94D-8B5A-66A9B06738AD}" name="Table2233" displayName="Table2233" ref="A158:B170" totalsRowShown="0">
-  <autoFilter ref="A158:B170" xr:uid="{ECF51F54-57EE-4277-8583-FC66BDE82BDE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="32" xr:uid="{A59002C8-F1F5-D94D-8B5A-66A9B06738AD}" name="Table2233" displayName="Table2233" ref="A160:B172" totalsRowShown="0">
+  <autoFilter ref="A160:B172" xr:uid="{ECF51F54-57EE-4277-8583-FC66BDE82BDE}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{FDBDC38E-C29F-C842-B0DF-BB9B4B41D86F}" name="Page for group: &quot;All points of interest&quot;"/>
     <tableColumn id="2" xr3:uid="{72470908-B945-E84A-B193-8B89B43D779D}" name="Column1"/>
@@ -588,8 +597,8 @@
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="33" xr:uid="{6B5CE5B3-EAE2-1C4E-BE3B-15B4434A7026}" name="Table2334" displayName="Table2334" ref="A172:B184" totalsRowShown="0">
-  <autoFilter ref="A172:B184" xr:uid="{17C4130F-4729-47ED-AFA7-C61CB4A33D00}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="33" xr:uid="{6B5CE5B3-EAE2-1C4E-BE3B-15B4434A7026}" name="Table2334" displayName="Table2334" ref="A174:B186" totalsRowShown="0">
+  <autoFilter ref="A174:B186" xr:uid="{17C4130F-4729-47ED-AFA7-C61CB4A33D00}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{A7644BBC-B281-C540-B1BF-0263A28CA359}" name="Page for group: &quot;All itineraries&quot;"/>
     <tableColumn id="2" xr3:uid="{A9C9CFE3-BF94-2E40-87D4-7C6DA54F1773}" name="Column1"/>
@@ -599,8 +608,8 @@
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{AD6838DD-4E69-3546-81FC-9C63610B1F7F}" name="Table2435" displayName="Table2435" ref="A186:B198" totalsRowShown="0">
-  <autoFilter ref="A186:B198" xr:uid="{4421B5D6-37B1-43A6-8C29-3894C8A06CEF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{AD6838DD-4E69-3546-81FC-9C63610B1F7F}" name="Table2435" displayName="Table2435" ref="A188:B200" totalsRowShown="0">
+  <autoFilter ref="A188:B200" xr:uid="{4421B5D6-37B1-43A6-8C29-3894C8A06CEF}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{1A2F8E68-4BDB-3B4A-8BDB-A1F6774D7E76}" name="Page for group: &quot;All services&quot;"/>
     <tableColumn id="2" xr3:uid="{47486761-2689-114D-9EB5-567D69EF092D}" name="Column1"/>
@@ -1000,8 +1009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7009AE2-141B-8F43-BF6B-7E6ECFF7233C}">
   <dimension ref="A1:A73"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1011,122 +1020,122 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
@@ -1141,7 +1150,7 @@
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
@@ -1166,7 +1175,7 @@
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
@@ -1191,7 +1200,7 @@
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
@@ -1201,12 +1210,12 @@
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
@@ -1221,7 +1230,7 @@
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
@@ -1236,7 +1245,7 @@
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
@@ -1251,7 +1260,7 @@
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
@@ -1266,7 +1275,7 @@
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
@@ -1281,7 +1290,7 @@
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
@@ -1296,7 +1305,7 @@
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
@@ -1311,7 +1320,7 @@
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1335,10 +1344,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D009084-A617-FE43-A7BE-1BA4673EB7A1}">
-  <dimension ref="A1:B198"/>
+  <dimension ref="A1:B200"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView zoomScale="114" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1349,10 +1358,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1360,90 +1369,90 @@
         <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -1451,15 +1460,15 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -1467,101 +1476,101 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B38" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -1574,7 +1583,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -1589,35 +1598,35 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B45" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -1627,39 +1636,39 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B53" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B55" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B57" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
@@ -1672,7 +1681,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -1687,35 +1696,35 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B62" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
@@ -1725,36 +1734,36 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B70" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B71" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B74" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
@@ -1767,7 +1776,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
@@ -1777,45 +1786,45 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B80" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
@@ -1825,31 +1834,31 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B88" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B89" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B91" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
@@ -1857,45 +1866,45 @@
         <v>23</v>
       </c>
       <c r="B92" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B94" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B99" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
@@ -1905,23 +1914,23 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B102" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B104" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
@@ -1929,69 +1938,69 @@
         <v>23</v>
       </c>
       <c r="B105" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B106" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B107" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B108" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B109" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B110" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B111" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B112" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B114" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B116" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
@@ -2004,466 +2013,479 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B118" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="B119" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B120" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>74</v>
+      </c>
       <c r="B121" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B122" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B123" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B124" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B125" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B126" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A127" t="s">
-        <v>77</v>
-      </c>
       <c r="B127" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B128" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A128" t="s">
-        <v>27</v>
-      </c>
-      <c r="B128" t="s">
-        <v>45</v>
+      <c r="B129" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B130" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>33</v>
+      </c>
+      <c r="B132" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A131" t="s">
-        <v>23</v>
-      </c>
-      <c r="B131" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B132" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>75</v>
+        <v>23</v>
       </c>
       <c r="B133" t="s">
-        <v>67</v>
+        <v>12</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B134" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>74</v>
+      </c>
       <c r="B135" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B136" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B137" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B138" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B139" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B140" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A141" t="s">
-        <v>77</v>
-      </c>
       <c r="B141" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B142" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A142" t="s">
-        <v>27</v>
-      </c>
-      <c r="B142" t="s">
-        <v>46</v>
+      <c r="B143" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B144" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A145" t="s">
-        <v>23</v>
-      </c>
-      <c r="B145" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>34</v>
+      </c>
       <c r="B146" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>75</v>
+        <v>23</v>
       </c>
       <c r="B147" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B148" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>74</v>
+      </c>
       <c r="B149" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B150" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B151" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B152" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B153" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B154" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A155" t="s">
-        <v>77</v>
-      </c>
       <c r="B155" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B156" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A156" t="s">
-        <v>27</v>
-      </c>
-      <c r="B156" t="s">
-        <v>46</v>
+      <c r="B157" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B158" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A159" t="s">
-        <v>23</v>
-      </c>
-      <c r="B159" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>35</v>
+      </c>
       <c r="B160" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>75</v>
+        <v>23</v>
       </c>
       <c r="B161" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B162" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>74</v>
+      </c>
       <c r="B163" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B164" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B165" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B166" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B167" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B168" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A169" t="s">
-        <v>77</v>
-      </c>
       <c r="B169" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B170" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A170" t="s">
-        <v>27</v>
-      </c>
-      <c r="B170" t="s">
-        <v>82</v>
+      <c r="B171" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B172" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A173" t="s">
-        <v>23</v>
-      </c>
-      <c r="B173" t="s">
-        <v>20</v>
+        <v>81</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>36</v>
+      </c>
       <c r="B174" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>75</v>
+        <v>23</v>
       </c>
       <c r="B175" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B176" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>74</v>
+      </c>
       <c r="B177" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B178" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B179" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B180" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B181" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B182" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A183" t="s">
-        <v>77</v>
-      </c>
       <c r="B183" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B184" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A184" t="s">
-        <v>27</v>
-      </c>
-      <c r="B184" t="s">
-        <v>83</v>
+      <c r="B185" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
+        <v>26</v>
+      </c>
+      <c r="B186" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>37</v>
+      </c>
+      <c r="B188" t="s">
         <v>38</v>
-      </c>
-      <c r="B186" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A187" t="s">
-        <v>23</v>
-      </c>
-      <c r="B187" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B188" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>75</v>
+        <v>23</v>
       </c>
       <c r="B189" t="s">
-        <v>67</v>
+        <v>22</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B190" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>74</v>
+      </c>
       <c r="B191" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B192" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B193" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B194" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B195" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B196" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A197" t="s">
-        <v>77</v>
-      </c>
       <c r="B197" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B198" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A198" t="s">
-        <v>27</v>
-      </c>
-      <c r="B198" t="s">
-        <v>47</v>
+      <c r="B199" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>26</v>
+      </c>
+      <c r="B200" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update excel and db schemas
</commit_message>
<xml_diff>
--- a/Design-part/UX diagram part A1 HYP design in the small and abstract pages.xlsx
+++ b/Design-part/UX diagram part A1 HYP design in the small and abstract pages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carloambrogi/Desktop/Hypermedia-Project/Design-part/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2692DAE-D0BF-BD4F-A84F-84727633F4DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7952E4-5AF6-5D4B-8F32-66731D7F0D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{CF35C348-60D3-C34C-B3F9-EC827BB88FFA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" activeTab="1" xr2:uid="{CF35C348-60D3-C34C-B3F9-EC827BB88FFA}"/>
   </bookViews>
   <sheets>
     <sheet name="Content tables" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="91">
   <si>
     <t>Kind of topic "Events"</t>
   </si>
@@ -306,6 +306,9 @@
   </si>
   <si>
     <t>Events</t>
+  </si>
+  <si>
+    <t>All events</t>
   </si>
 </sst>
 </file>
@@ -537,8 +540,8 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="29" xr:uid="{55FEF2F9-6341-C247-9487-CFEFD17FCE16}" name="Table1930" displayName="Table1930" ref="A110:B123" totalsRowShown="0">
-  <autoFilter ref="A110:B123" xr:uid="{E3E927A6-B68F-4E61-A3D7-F69689C11112}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="29" xr:uid="{55FEF2F9-6341-C247-9487-CFEFD17FCE16}" name="Table1930" displayName="Table1930" ref="A110:B125" totalsRowShown="0">
+  <autoFilter ref="A110:B125" xr:uid="{E3E927A6-B68F-4E61-A3D7-F69689C11112}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{8D4B2448-8015-7C45-B908-ED9EC8D412BA}" name="Page for group: &quot;All events&quot;"/>
     <tableColumn id="2" xr3:uid="{7FC86B2C-B2EA-5B45-8407-382B9ECCC1D8}" name="Column1"/>
@@ -548,8 +551,8 @@
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="30" xr:uid="{A227AA2E-5D6D-0348-A268-39F0C01F1493}" name="Table2031" displayName="Table2031" ref="A125:B136" totalsRowShown="0">
-  <autoFilter ref="A125:B136" xr:uid="{950BC4F7-D3EE-499C-93A7-A5E79CEC86F6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="30" xr:uid="{A227AA2E-5D6D-0348-A268-39F0C01F1493}" name="Table2031" displayName="Table2031" ref="A127:B140" totalsRowShown="0">
+  <autoFilter ref="A127:B140" xr:uid="{950BC4F7-D3EE-499C-93A7-A5E79CEC86F6}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{361A93E6-9656-B14D-8C82-3BA6F871E2A9}" name="Page for group: &quot;All summer events&quot;"/>
     <tableColumn id="2" xr3:uid="{8AD30F5A-AC89-2D46-B527-A99E6E56A427}" name="Group &quot;All summer events&quot;"/>
@@ -569,8 +572,8 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="31" xr:uid="{31713721-7F1E-9B40-9FAD-E5E0012F8CED}" name="Table2132" displayName="Table2132" ref="A138:B149" totalsRowShown="0">
-  <autoFilter ref="A138:B149" xr:uid="{47676A86-326F-4B55-8642-E1FA72DA0872}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="31" xr:uid="{31713721-7F1E-9B40-9FAD-E5E0012F8CED}" name="Table2132" displayName="Table2132" ref="A142:B155" totalsRowShown="0">
+  <autoFilter ref="A142:B155" xr:uid="{47676A86-326F-4B55-8642-E1FA72DA0872}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{40C615F9-7C3C-4F42-9F21-D9DDC9A72D6C}" name="Page for group: &quot;All winter events&quot;"/>
     <tableColumn id="2" xr3:uid="{D8ED8285-E648-1047-87D8-C3D5B6509C40}" name="Column1"/>
@@ -580,8 +583,8 @@
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="32" xr:uid="{A59002C8-F1F5-D94D-8B5A-66A9B06738AD}" name="Table2233" displayName="Table2233" ref="A151:B162" totalsRowShown="0">
-  <autoFilter ref="A151:B162" xr:uid="{ECF51F54-57EE-4277-8583-FC66BDE82BDE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="32" xr:uid="{A59002C8-F1F5-D94D-8B5A-66A9B06738AD}" name="Table2233" displayName="Table2233" ref="A157:B168" totalsRowShown="0">
+  <autoFilter ref="A157:B168" xr:uid="{ECF51F54-57EE-4277-8583-FC66BDE82BDE}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{FDBDC38E-C29F-C842-B0DF-BB9B4B41D86F}" name="Page for group: &quot;All points of interest&quot;"/>
     <tableColumn id="2" xr3:uid="{72470908-B945-E84A-B193-8B89B43D779D}" name="Column1"/>
@@ -591,8 +594,8 @@
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="33" xr:uid="{6B5CE5B3-EAE2-1C4E-BE3B-15B4434A7026}" name="Table2334" displayName="Table2334" ref="A164:B175" totalsRowShown="0">
-  <autoFilter ref="A164:B175" xr:uid="{17C4130F-4729-47ED-AFA7-C61CB4A33D00}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="33" xr:uid="{6B5CE5B3-EAE2-1C4E-BE3B-15B4434A7026}" name="Table2334" displayName="Table2334" ref="A170:B181" totalsRowShown="0">
+  <autoFilter ref="A170:B181" xr:uid="{17C4130F-4729-47ED-AFA7-C61CB4A33D00}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{A7644BBC-B281-C540-B1BF-0263A28CA359}" name="Page for group: &quot;All itineraries&quot;"/>
     <tableColumn id="2" xr3:uid="{A9C9CFE3-BF94-2E40-87D4-7C6DA54F1773}" name="Column1"/>
@@ -602,8 +605,8 @@
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{AD6838DD-4E69-3546-81FC-9C63610B1F7F}" name="Table2435" displayName="Table2435" ref="A177:B188" totalsRowShown="0">
-  <autoFilter ref="A177:B188" xr:uid="{4421B5D6-37B1-43A6-8C29-3894C8A06CEF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{AD6838DD-4E69-3546-81FC-9C63610B1F7F}" name="Table2435" displayName="Table2435" ref="A183:B194" totalsRowShown="0">
+  <autoFilter ref="A183:B194" xr:uid="{4421B5D6-37B1-43A6-8C29-3894C8A06CEF}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{1A2F8E68-4BDB-3B4A-8BDB-A1F6774D7E76}" name="Page for group: &quot;All services&quot;"/>
     <tableColumn id="2" xr3:uid="{47486761-2689-114D-9EB5-567D69EF092D}" name="Column1"/>
@@ -1003,7 +1006,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7009AE2-141B-8F43-BF6B-7E6ECFF7233C}">
   <dimension ref="A1:A73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1338,10 +1341,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D009084-A617-FE43-A7BE-1BA4673EB7A1}">
-  <dimension ref="A1:B188"/>
+  <dimension ref="A1:B194"/>
   <sheetViews>
-    <sheetView zoomScale="114" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A129" zoomScale="114" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A154" sqref="A154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2023,366 +2026,396 @@
         <v>26</v>
       </c>
       <c r="B123" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B124" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B125" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A125" t="s">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
         <v>33</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B127" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A126" t="s">
-        <v>23</v>
-      </c>
-      <c r="B126" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B127" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>74</v>
+        <v>23</v>
       </c>
       <c r="B128" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B129" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>74</v>
+      </c>
       <c r="B130" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B131" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B132" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B133" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B134" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B135" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B136" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B137" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A136" t="s">
-        <v>26</v>
-      </c>
-      <c r="B136" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B138" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A139" t="s">
-        <v>23</v>
-      </c>
       <c r="B139" t="s">
-        <v>16</v>
+        <v>88</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B140" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A141" t="s">
-        <v>74</v>
-      </c>
-      <c r="B141" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>34</v>
+      </c>
       <c r="B142" t="s">
-        <v>89</v>
+        <v>38</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>23</v>
+      </c>
       <c r="B143" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B144" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>74</v>
+      </c>
       <c r="B145" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B146" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B147" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B148" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B149" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B150" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B151" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B152" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A149" t="s">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
         <v>26</v>
       </c>
-      <c r="B149" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A151" t="s">
-        <v>35</v>
-      </c>
-      <c r="B151" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A152" t="s">
-        <v>23</v>
-      </c>
-      <c r="B152" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B153" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A154" t="s">
-        <v>74</v>
-      </c>
       <c r="B154" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B155" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B156" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>35</v>
+      </c>
       <c r="B157" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>23</v>
+      </c>
       <c r="B158" t="s">
-        <v>69</v>
+        <v>18</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B159" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>74</v>
+      </c>
       <c r="B160" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B161" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A162" t="s">
-        <v>26</v>
-      </c>
       <c r="B162" t="s">
-        <v>79</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B163" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A164" t="s">
-        <v>36</v>
-      </c>
       <c r="B164" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A165" t="s">
-        <v>23</v>
-      </c>
       <c r="B165" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B166" t="s">
-        <v>64</v>
+        <v>25</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A167" t="s">
-        <v>74</v>
-      </c>
       <c r="B167" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>26</v>
+      </c>
       <c r="B168" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B169" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>36</v>
+      </c>
       <c r="B170" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>23</v>
+      </c>
       <c r="B171" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B172" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>74</v>
+      </c>
       <c r="B173" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B174" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A175" t="s">
-        <v>26</v>
-      </c>
       <c r="B175" t="s">
-        <v>80</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B176" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A177" t="s">
-        <v>37</v>
-      </c>
       <c r="B177" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A178" t="s">
-        <v>23</v>
-      </c>
       <c r="B178" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B179" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A180" t="s">
-        <v>74</v>
-      </c>
       <c r="B180" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>26</v>
+      </c>
       <c r="B181" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B182" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>37</v>
+      </c>
       <c r="B183" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>23</v>
+      </c>
       <c r="B184" t="s">
-        <v>69</v>
+        <v>22</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B185" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>74</v>
+      </c>
       <c r="B186" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B187" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B188" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B189" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B190" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B191" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B192" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B193" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A188" t="s">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
         <v>26</v>
       </c>
-      <c r="B188" t="s">
+      <c r="B194" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>